<commit_message>
Updated models. Created results figure production files. Added results figures and spreadsheets.
</commit_message>
<xml_diff>
--- a/data/species_dist.xlsx
+++ b/data/species_dist.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\GitHub\Transpiration-ML-Project\Transpiration-ML-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09895F86-956A-4762-9C23-A8B0F47DFE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE574445-0652-4AC0-ACBD-24818A89C692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_dist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -691,37 +702,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -1562,16 +1543,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -2470,16 +2451,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2807,7 +2788,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add mixed forest data cluster
</commit_message>
<xml_diff>
--- a/data/species_dist.xlsx
+++ b/data/species_dist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\GitHub\Transpiration-ML-Project\Transpiration-ML-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE574445-0652-4AC0-ACBD-24818A89C692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4053642-AE1F-47C0-A143-F9EDBCD45278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Count</t>
   </si>
@@ -45,106 +45,280 @@
     <t>Eucalyptus tereticornis</t>
   </si>
   <si>
+    <t>Pinus strobus</t>
+  </si>
+  <si>
+    <t>Picea abies</t>
+  </si>
+  <si>
+    <t>Fagus sylvatica</t>
+  </si>
+  <si>
+    <t>Quercus ilex</t>
+  </si>
+  <si>
+    <t>Olea europaea</t>
+  </si>
+  <si>
+    <t>Pinus sylvestris</t>
+  </si>
+  <si>
+    <t>Betula pubescens subsp. czerepanovii</t>
+  </si>
+  <si>
+    <t>Picea sitchensis</t>
+  </si>
+  <si>
+    <t>Elaeis guineensis</t>
+  </si>
+  <si>
+    <t>Hevea brasiliensis</t>
+  </si>
+  <si>
+    <t>Pinus halepensis</t>
+  </si>
+  <si>
+    <t>Larix decidua</t>
+  </si>
+  <si>
+    <t>Agathis australis</t>
+  </si>
+  <si>
+    <t>Quercus suber</t>
+  </si>
+  <si>
+    <t>Acacia tortilis</t>
+  </si>
+  <si>
+    <t>Liriodendron tulipifera</t>
+  </si>
+  <si>
+    <t>Pinus taeda</t>
+  </si>
+  <si>
+    <t>Picea glauca</t>
+  </si>
+  <si>
+    <t>Liquidambar styraciflua</t>
+  </si>
+  <si>
+    <t>Populus canescens</t>
+  </si>
+  <si>
+    <t>Malus domestica</t>
+  </si>
+  <si>
+    <t>Pinus sibirica</t>
+  </si>
+  <si>
+    <t>Ostrya virginiana</t>
+  </si>
+  <si>
+    <t>Quercus phellos</t>
+  </si>
+  <si>
+    <t>Juniperus monosperma</t>
+  </si>
+  <si>
+    <t>Carpinus betulus</t>
+  </si>
+  <si>
+    <t>Carapa guianensis</t>
+  </si>
+  <si>
+    <t>Eucalyptus rubida</t>
+  </si>
+  <si>
+    <t>Goupia glabra</t>
+  </si>
+  <si>
+    <t>Quercus rubra</t>
+  </si>
+  <si>
+    <t>Pinus rigida</t>
+  </si>
+  <si>
+    <t>Fagus grandifolia</t>
+  </si>
+  <si>
+    <t>Betula pubescens</t>
+  </si>
+  <si>
+    <t>Pinus virginiana</t>
+  </si>
+  <si>
+    <t>Quercus coccinea</t>
+  </si>
+  <si>
+    <t>Pinus cembra</t>
+  </si>
+  <si>
+    <t>Ulmus americana</t>
+  </si>
+  <si>
+    <t>Quercus faginea</t>
+  </si>
+  <si>
+    <t>Prunus serotina</t>
+  </si>
+  <si>
+    <t>Quercus spp.</t>
+  </si>
+  <si>
+    <t>Recordoxylon speciosum</t>
+  </si>
+  <si>
+    <t>Dicorynia guianensis</t>
+  </si>
+  <si>
     <t>Eucalyptus obliqua</t>
   </si>
   <si>
-    <t>Pinus strobus</t>
-  </si>
-  <si>
-    <t>Picea abies</t>
+    <t>Eschweillera sp.</t>
+  </si>
+  <si>
+    <t>Sassafras albidum</t>
+  </si>
+  <si>
+    <t>Mortoniodendron anisophyllum</t>
+  </si>
+  <si>
+    <t>Oxandra asbeckii</t>
+  </si>
+  <si>
+    <t>Betula alleghaniensis</t>
+  </si>
+  <si>
+    <t>Cupania macrophylla</t>
+  </si>
+  <si>
+    <t>Tsuga canadensis</t>
+  </si>
+  <si>
+    <t>Fraxinus excelsior</t>
+  </si>
+  <si>
+    <t>Gymnanthes riparia</t>
+  </si>
+  <si>
+    <t>Quercus pubescens</t>
+  </si>
+  <si>
+    <t>Aspidosperma desmanthum</t>
+  </si>
+  <si>
+    <t>Inga sp.</t>
+  </si>
+  <si>
+    <t>Iryanthera sagotiana</t>
+  </si>
+  <si>
+    <t>Pinus edulis</t>
+  </si>
+  <si>
+    <t>Fraxinus americana</t>
+  </si>
+  <si>
+    <t>Quercus michauxii</t>
+  </si>
+  <si>
+    <t>Pleuranthodendron lindenii</t>
+  </si>
+  <si>
+    <t>Meliosma idiopoda</t>
+  </si>
+  <si>
+    <t>Acer saccharum</t>
+  </si>
+  <si>
+    <t>Sloanea sp</t>
+  </si>
+  <si>
+    <t>Quercus velutina</t>
+  </si>
+  <si>
+    <t>Genipa americana</t>
+  </si>
+  <si>
+    <t>Larix sibirica Ledeb.</t>
+  </si>
+  <si>
+    <t>Quercus montana</t>
+  </si>
+  <si>
+    <t>Licania membranacea</t>
+  </si>
+  <si>
+    <t>Pouteria sp.</t>
+  </si>
+  <si>
+    <t>Quercus prinus</t>
+  </si>
+  <si>
+    <t>Trophis mexicana</t>
+  </si>
+  <si>
+    <t>Brosimum alicastrum</t>
+  </si>
+  <si>
+    <t>Quercus robur</t>
+  </si>
+  <si>
+    <t>Pinus nigra</t>
+  </si>
+  <si>
+    <t>Vacapoua americana</t>
+  </si>
+  <si>
+    <t>Macrolobium costaricense</t>
   </si>
   <si>
     <t>Pouteria viridis</t>
   </si>
   <si>
-    <t>Quercus robur</t>
-  </si>
-  <si>
-    <t>Fagus sylvatica</t>
-  </si>
-  <si>
-    <t>Pinus nigra</t>
-  </si>
-  <si>
-    <t>Quercus ilex</t>
-  </si>
-  <si>
-    <t>Olea europaea</t>
-  </si>
-  <si>
-    <t>Pinus sylvestris</t>
-  </si>
-  <si>
-    <t>Betula pubescens subsp. czerepanovii</t>
-  </si>
-  <si>
-    <t>Picea sitchensis</t>
-  </si>
-  <si>
-    <t>Sloanea sp</t>
-  </si>
-  <si>
-    <t>Dicorynia guianensis</t>
-  </si>
-  <si>
-    <t>Elaeis guineensis</t>
-  </si>
-  <si>
-    <t>Hevea brasiliensis</t>
-  </si>
-  <si>
-    <t>Pinus halepensis</t>
-  </si>
-  <si>
-    <t>Larix decidua</t>
-  </si>
-  <si>
-    <t>Agathis australis</t>
-  </si>
-  <si>
-    <t>Quercus suber</t>
-  </si>
-  <si>
-    <t>Larix sibirica Ledeb.</t>
-  </si>
-  <si>
-    <t>Acacia tortilis</t>
-  </si>
-  <si>
-    <t>Liriodendron tulipifera</t>
-  </si>
-  <si>
-    <t>Pinus taeda</t>
-  </si>
-  <si>
-    <t>Picea glauca</t>
-  </si>
-  <si>
-    <t>Acer saccharum</t>
-  </si>
-  <si>
-    <t>Liquidambar styraciflua</t>
-  </si>
-  <si>
-    <t>Pinus edulis</t>
-  </si>
-  <si>
-    <t>Quercus montana</t>
-  </si>
-  <si>
-    <t>Betula alleghaniensis</t>
+    <t>Tilia americana</t>
+  </si>
+  <si>
+    <t>Betula papyrifera</t>
+  </si>
+  <si>
+    <t>Quercus falcata</t>
+  </si>
+  <si>
+    <t>Cornus florida</t>
+  </si>
+  <si>
+    <t>Carya tomentosa</t>
+  </si>
+  <si>
+    <t>Otoba novogranatensis</t>
+  </si>
+  <si>
+    <t>Arbutus unedo</t>
+  </si>
+  <si>
+    <t>Fraxinus pennsylvanica</t>
+  </si>
+  <si>
+    <t>Vantanea sp</t>
+  </si>
+  <si>
+    <t>Populus grandidentata</t>
   </si>
   <si>
     <t>Acer rubrum</t>
   </si>
   <si>
-    <t>Fraxinus pennsylvanica</t>
-  </si>
-  <si>
-    <t>Populus canescens</t>
-  </si>
-  <si>
-    <t>Malus domestica</t>
+    <t>Ampelocera macrocarpa</t>
+  </si>
+  <si>
+    <t>Vouacapoua americana</t>
+  </si>
+  <si>
+    <t>Larix gmelinii</t>
+  </si>
+  <si>
+    <t>Quercus alba</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1702,1461 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="37"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-4600-4BC0-B27B-9CD4454B10DC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="38"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004C-4600-4BC0-B27B-9CD4454B10DC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="39"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-4600-4BC0-B27B-9CD4454B10DC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="40"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004E-4600-4BC0-B27B-9CD4454B10DC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="41"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-4600-4BC0-B27B-9CD4454B10DC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="42"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="44"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="45"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="46"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="47"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-268C-4AAE-B2F9-6D92ED460691}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="48"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="49"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="50"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="51"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="52"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="53"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="54"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="55"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="56"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="57"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="58"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="59"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="60"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="61"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="62"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="63"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-268C-4AAE-B2F9-6D92ED460691}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="64"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000056-268C-4AAE-B2F9-6D92ED460691}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="65"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="66"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="67"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="68"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="69"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="70"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="71"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="72"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="73"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="74"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="75"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="76"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="77"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="78"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="79"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="80"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="81"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="82"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="83"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="84"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="85"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="86"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-268C-4AAE-B2F9-6D92ED460691}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="87"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000058-268C-4AAE-B2F9-6D92ED460691}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="88"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="89"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="90"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="91"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="92"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="93"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="94"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-65D9-4F67-85DF-6BE3499864ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-65D9-4F67-85DF-6BE3499864ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-65D9-4F67-85DF-6BE3499864ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.1305932692339764E-3"/>
+                  <c:y val="3.5094873395945102E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-65D9-4F67-85DF-6BE3499864ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="30"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000003D-65D9-4F67-85DF-6BE3499864ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="35"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.7466341167328674E-2"/>
+                  <c:y val="2.3329825081701522E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000047-65D9-4F67-85DF-6BE3499864ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="47"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000057-268C-4AAE-B2F9-6D92ED460691}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="63"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000059-268C-4AAE-B2F9-6D92ED460691}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="64"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000056-268C-4AAE-B2F9-6D92ED460691}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="86"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000055-268C-4AAE-B2F9-6D92ED460691}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="87"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000058-268C-4AAE-B2F9-6D92ED460691}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1543,7 +3171,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1585,134 +3213,308 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>species_dist!$A$2:$A$38</c:f>
+              <c:f>species_dist!$A$2:$A$96</c:f>
               <c:strCache>
-                <c:ptCount val="37"/>
+                <c:ptCount val="95"/>
                 <c:pt idx="0">
+                  <c:v>Carpinus betulus</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Quercus spp.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Recordoxylon speciosum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dicorynia guianensis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Eucalyptus obliqua</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Eschweillera sp.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sassafras albidum</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Quercus rubra</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Mortoniodendron anisophyllum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oxandra asbeckii</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Picea glauca</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Picea sitchensis</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Pinus rigida</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Betula alleghaniensis</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Cupania macrophylla</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Tsuga canadensis</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Fraxinus excelsior</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Gymnanthes riparia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Populus canescens</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Quercus pubescens</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Aspidosperma desmanthum</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Elaeis guineensis</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Nothofagus pumilio</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="23">
+                  <c:v>Inga sp.</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Iryanthera sagotiana</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Pinus sibirica</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Quercus faginea</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Pinus edulis</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Liquidambar styraciflua</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Fagus sylvatica</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Hevea brasiliensis</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Fraxinus americana</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Quercus michauxii</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Eucalyptus tereticornis</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Goupia glabra</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Pleuranthodendron lindenii</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Meliosma idiopoda</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Acer saccharum</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Sloanea sp</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Ostrya virginiana</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Quercus velutina</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Agathis australis</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Genipa americana</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Larix sibirica Ledeb.</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Quercus montana</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Betula pubescens</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Licania membranacea</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Pinus sylvestris</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Pouteria sp.</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Quercus prinus</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Trophis mexicana</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Brosimum alicastrum</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Quercus robur</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Pinus nigra</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Vacapoua americana</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Pinus virginiana</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Macrolobium costaricense</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>Nothofagus antarctica</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Eucalyptus tereticornis</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Eucalyptus obliqua</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="58">
+                  <c:v>Quercus coccinea</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Pouteria viridis</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Tilia americana</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Prunus serotina</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>Betula papyrifera</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>Larix decidua</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Liriodendron tulipifera</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Quercus falcata</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Acacia tortilis</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Olea europaea</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>Carapa guianensis</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Ulmus americana</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>Cornus florida</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>Carya tomentosa</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>Eucalyptus rubida</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>Otoba novogranatensis</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>Arbutus unedo</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>Betula pubescens subsp. czerepanovii</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>Fraxinus pennsylvanica</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>Vantanea sp</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>Populus grandidentata</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>Acer rubrum</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>Malus domestica</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>Ampelocera macrocarpa</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>Vouacapoua americana</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>Quercus suber</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>Larix gmelinii</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>Juniperus monosperma</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>Picea abies</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>Quercus alba</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>Quercus phellos</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>Pinus halepensis</c:v>
+                </c:pt>
+                <c:pt idx="90">
                   <c:v>Pinus strobus</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Picea abies</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Pouteria viridis</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Quercus robur</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Fagus sylvatica</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Pinus nigra</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="91">
+                  <c:v>Pinus taeda</c:v>
+                </c:pt>
+                <c:pt idx="92">
                   <c:v>Quercus ilex</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Olea europaea</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pinus sylvestris</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Betula pubescens subsp. czerepanovii</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Picea sitchensis</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Sloanea sp</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Dicorynia guianensis</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Elaeis guineensis</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Hevea brasiliensis</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pinus halepensis</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Larix decidua</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Agathis australis</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Quercus suber</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Larix sibirica Ledeb.</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Acacia tortilis</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Liriodendron tulipifera</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Pinus taeda</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Picea glauca</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Acer saccharum</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Liquidambar styraciflua</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Pinus edulis</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Quercus montana</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Betula alleghaniensis</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Acer rubrum</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Fraxinus pennsylvanica</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Populus canescens</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Malus domestica</c:v>
+                <c:pt idx="93">
+                  <c:v>Pinus cembra</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>Fagus grandifolia</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>species_dist!$B$2:$B$38</c:f>
+              <c:f>species_dist!$B$2:$B$96</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="95"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1721,102 +3523,276 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="28">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="87">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="88">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="89">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="90">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="92">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="93">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="94">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2451,16 +4427,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2785,10 +4761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2803,7 +4779,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2811,15 +4787,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2827,7 +4803,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2835,23 +4811,23 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2859,55 +4835,55 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2915,7 +4891,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2923,7 +4899,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2931,7 +4907,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2939,7 +4915,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2947,15 +4923,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2963,15 +4939,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2979,7 +4955,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2987,7 +4963,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2995,15 +4971,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3011,55 +4987,55 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3067,23 +5043,23 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3091,9 +5067,473 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>95</v>
+      </c>
+      <c r="B89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>27</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96">
         <v>2</v>
       </c>
     </row>

</xml_diff>